<commit_message>
added in iteration for each item in ProductOrder.xlsx, haven't been able to fully test as server for website crashed
</commit_message>
<xml_diff>
--- a/Project2/ProductOrders.xlsx
+++ b/Project2/ProductOrders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stuff\Revature\sy-project-2\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C692AC9-596F-4891-8FAD-43580FF3A407}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BC0CEA-85E0-4ED8-9C5B-707BE1CA135E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7530" activeTab="1" xr2:uid="{803B3F17-6292-4F8B-B785-946992B28C49}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7530" firstSheet="1" activeTab="1" xr2:uid="{803B3F17-6292-4F8B-B785-946992B28C49}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
did slight work on Product Ordering
</commit_message>
<xml_diff>
--- a/Project2/ProductOrders.xlsx
+++ b/Project2/ProductOrders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stuff\Revature\sy-project-2\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB4E103-F7F3-4E37-AE1F-5DDC2B7FB140}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE028EB-D479-47E0-8F3F-C58C033F95CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7530" xr2:uid="{803B3F17-6292-4F8B-B785-946992B28C49}"/>
   </bookViews>
@@ -97,10 +97,10 @@
     <t>Primary Phone</t>
   </si>
   <si>
+    <t>Ipoh Coff</t>
+  </si>
+  <si>
     <t>Succeeded</t>
-  </si>
-  <si>
-    <t>Ipoh Coff</t>
   </si>
   <si>
     <t>Failed</t>
@@ -490,7 +490,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -512,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,7 +534,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -556,12 +556,12 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>4</v>

</xml_diff>

<commit_message>
using project2 to help test logic for project3, mostly email invoice logic
</commit_message>
<xml_diff>
--- a/Project2/ProductOrders.xlsx
+++ b/Project2/ProductOrders.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stuff\Revature\sy-project-2\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD67E2D-7103-4C81-B712-E39D7547984C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34801D88-7B99-4E20-BF26-8F3F770B87EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3810" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{803B3F17-6292-4F8B-B785-946992B28C49}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{803B3F17-6292-4F8B-B785-946992B28C49}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="2" r:id="rId1"/>
     <sheet name="Address" sheetId="3" r:id="rId2"/>
+    <sheet name="Invoice" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Chai</t>
   </si>
@@ -103,19 +104,55 @@
     <t>Succeeded</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>Item out of stock or doesn't exist.</t>
-  </si>
-  <si>
-    <t>Order #512743</t>
+    <t>UnitPrice</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>$10.00</t>
+  </si>
+  <si>
+    <t>$23.00</t>
+  </si>
+  <si>
+    <t>$7.00</t>
+  </si>
+  <si>
+    <t>$7.50</t>
+  </si>
+  <si>
+    <t>$2.25</t>
+  </si>
+  <si>
+    <t>$9.00</t>
+  </si>
+  <si>
+    <t>$20.00</t>
+  </si>
+  <si>
+    <t>$69.00</t>
+  </si>
+  <si>
+    <t>$28.00</t>
+  </si>
+  <si>
+    <t>$4.50</t>
+  </si>
+  <si>
+    <t>$90.00</t>
+  </si>
+  <si>
+    <t>$14.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,8 +182,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41329632-D687-4E24-927D-FDEA825D4A51}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,9 +536,6 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -512,9 +547,6 @@
       <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -526,9 +558,6 @@
       <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -540,9 +569,6 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -554,9 +580,6 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -568,9 +591,6 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -582,9 +602,6 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -592,12 +609,6 @@
       </c>
       <c r="B9">
         <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -666,4 +677,137 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73BAD1B-F1CB-474F-B9A5-22611EEC1514}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>